<commit_message>
New benchmark with postal code
</commit_message>
<xml_diff>
--- a/Ergebnisse für Google.xlsx
+++ b/Ergebnisse für Google.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Ergebnisse für Google" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2183" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="381">
   <si>
     <t>PLZ</t>
   </si>
@@ -1957,13 +1957,13 @@
   <dimension ref="A1:M1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="12" max="12" width="20.75" customWidth="1"/>
-    <col min="13" max="13" width="17.375" customWidth="1"/>
+    <col min="12" max="12" width="18.625" customWidth="1"/>
+    <col min="13" max="13" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -2015,20 +2015,20 @@
         <v>47.372705189999998</v>
       </c>
       <c r="G2">
-        <v>8.4129387999999992</v>
+        <v>8.4498192999999997</v>
       </c>
       <c r="H2">
-        <v>47.398938299999998</v>
+        <v>47.371437299999997</v>
       </c>
       <c r="I2">
-        <v>4869.2700000000004</v>
+        <v>228.24</v>
       </c>
       <c r="L2" t="s">
         <v>377</v>
       </c>
       <c r="M2" s="1">
         <f>COUNTIF(I2:I1001,"&lt;=20")</f>
-        <v>673</v>
+        <v>783</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -2051,20 +2051,20 @@
         <v>47.373550450000003</v>
       </c>
       <c r="G3">
-        <v>8.4234141999999999</v>
+        <v>8.4487427999999998</v>
       </c>
       <c r="H3">
-        <v>47.390861999999998</v>
+        <v>47.373533199999997</v>
       </c>
       <c r="I3">
-        <v>3370.51</v>
+        <v>36.630000000000003</v>
       </c>
       <c r="L3" t="s">
         <v>378</v>
       </c>
       <c r="M3" s="2">
         <f>COUNT(I2:I1001)-COUNTIF(I2:I1001,"&lt;=20")-COUNTIF(I2:I1001,"&gt;100")</f>
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -2100,7 +2100,7 @@
       </c>
       <c r="M4" s="3">
         <f>COUNTIF(I2:I1001,"&gt;100")</f>
-        <v>195</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -2136,7 +2136,7 @@
       </c>
       <c r="M5">
         <f>1000-M2-M3-M4</f>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -2188,13 +2188,13 @@
         <v>47.396477869999998</v>
       </c>
       <c r="G7">
-        <v>8.5446112999999997</v>
+        <v>8.4487548999999902</v>
       </c>
       <c r="H7">
-        <v>47.408263099999999</v>
+        <v>47.396543899999998</v>
       </c>
       <c r="I7">
-        <v>10741.75</v>
+        <v>7.35</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -2275,13 +2275,13 @@
         <v>47.404680939999999</v>
       </c>
       <c r="G10">
-        <v>8.4787438999999996</v>
+        <v>8.4490277999999996</v>
       </c>
       <c r="H10">
-        <v>47.338052900000001</v>
+        <v>47.404646</v>
       </c>
       <c r="I10">
-        <v>8040.08</v>
+        <v>4.5199999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -2304,13 +2304,13 @@
         <v>47.405769839999998</v>
       </c>
       <c r="G11">
-        <v>8.5373377999999995</v>
+        <v>8.4488368000000005</v>
       </c>
       <c r="H11">
-        <v>47.380418599999999</v>
+        <v>47.405753999999902</v>
       </c>
       <c r="I11">
-        <v>10226.6</v>
+        <v>5.27</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -2333,13 +2333,13 @@
         <v>47.406274500000002</v>
       </c>
       <c r="G12">
-        <v>8.537369</v>
+        <v>8.4490052999999996</v>
       </c>
       <c r="H12">
-        <v>47.380400399999999</v>
+        <v>47.406256300000003</v>
       </c>
       <c r="I12">
-        <v>10227.629999999999</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -2594,13 +2594,13 @@
         <v>47.396528580000002</v>
       </c>
       <c r="G21">
-        <v>8.5444260999999901</v>
+        <v>8.4491260999999902</v>
       </c>
       <c r="H21">
-        <v>47.408434399999997</v>
+        <v>47.3965587</v>
       </c>
       <c r="I21">
-        <v>10672.7</v>
+        <v>8.82</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2623,13 +2623,13 @@
         <v>47.397161840000003</v>
       </c>
       <c r="G22">
-        <v>8.5625228</v>
+        <v>8.4499049999999993</v>
       </c>
       <c r="H22">
-        <v>47.366424799999997</v>
+        <v>47.397126800000002</v>
       </c>
       <c r="I22">
-        <v>12977.98</v>
+        <v>5.08</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -2655,7 +2655,7 @@
         <v>8.4488272000000002</v>
       </c>
       <c r="H23">
-        <v>47.397394200000001</v>
+        <v>47.397394299999903</v>
       </c>
       <c r="I23">
         <v>21.24</v>
@@ -2710,13 +2710,13 @@
         <v>47.397335630000001</v>
       </c>
       <c r="G25">
-        <v>8.4500306999999992</v>
+        <v>8.45006729999999</v>
       </c>
       <c r="H25">
-        <v>47.397396000000001</v>
+        <v>47.397395099999997</v>
       </c>
       <c r="I25">
-        <v>7.56</v>
+        <v>6.56</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -2768,13 +2768,13 @@
         <v>47.400802110000001</v>
       </c>
       <c r="G27">
-        <v>8.5611636000000004</v>
+        <v>8.4502215999999901</v>
       </c>
       <c r="H27">
-        <v>47.368934499999902</v>
+        <v>47.400533899999999</v>
       </c>
       <c r="I27">
-        <v>12842.29</v>
+        <v>32.880000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -2884,13 +2884,13 @@
         <v>47.406465019999999</v>
       </c>
       <c r="G31">
-        <v>8.5142451000000001</v>
+        <v>8.4495123000000003</v>
       </c>
       <c r="H31">
-        <v>47.3965149</v>
+        <v>47.406440699999997</v>
       </c>
       <c r="I31">
-        <v>7280.45</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2913,13 +2913,13 @@
         <v>47.406164820000001</v>
       </c>
       <c r="G32">
-        <v>8.5373020999999998</v>
+        <v>8.4495731999999997</v>
       </c>
       <c r="H32">
-        <v>47.380438899999902</v>
+        <v>47.406161400000002</v>
       </c>
       <c r="I32">
-        <v>10155.14</v>
+        <v>5.27</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -2942,13 +2942,13 @@
         <v>47.410502729999997</v>
       </c>
       <c r="G33">
-        <v>8.5277767000000004</v>
+        <v>8.4495618999999902</v>
       </c>
       <c r="H33">
-        <v>47.390684</v>
+        <v>47.410451999999999</v>
       </c>
       <c r="I33">
-        <v>8939.58</v>
+        <v>30.7</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3087,13 +3087,13 @@
         <v>47.413765329999997</v>
       </c>
       <c r="G38">
-        <v>8.4498354999999901</v>
+        <v>8.4498131999999995</v>
       </c>
       <c r="H38">
-        <v>47.413583499999902</v>
+        <v>47.413575299999998</v>
       </c>
       <c r="I38">
-        <v>42.42</v>
+        <v>45.04</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -3116,13 +3116,13 @@
         <v>47.370401200000003</v>
       </c>
       <c r="G39">
-        <v>8.4583449000000002</v>
+        <v>8.4506025000000005</v>
       </c>
       <c r="H39">
-        <v>47.397880899999997</v>
+        <v>47.370370399999999</v>
       </c>
       <c r="I39">
-        <v>3144.93</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3145,13 +3145,13 @@
         <v>47.370824079999998</v>
       </c>
       <c r="G40">
-        <v>8.4135998999999995</v>
+        <v>8.4510592999999901</v>
       </c>
       <c r="H40">
-        <v>47.399269399999902</v>
+        <v>47.370717199999902</v>
       </c>
       <c r="I40">
-        <v>5204.1899999999996</v>
+        <v>14.63</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -3348,13 +3348,13 @@
         <v>47.395323750000003</v>
       </c>
       <c r="G47">
-        <v>8.4259672999999999</v>
+        <v>8.4505198999999998</v>
       </c>
       <c r="H47">
-        <v>47.389257099999902</v>
+        <v>47.395314200000001</v>
       </c>
       <c r="I47">
-        <v>2822.07</v>
+        <v>11.07</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -3406,13 +3406,13 @@
         <v>47.397090400000003</v>
       </c>
       <c r="G49">
-        <v>8.4505740999999901</v>
+        <v>8.4505792</v>
       </c>
       <c r="H49">
-        <v>47.397052899999998</v>
+        <v>47.397040699999998</v>
       </c>
       <c r="I49">
-        <v>5.08</v>
+        <v>6.51</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -3435,13 +3435,13 @@
         <v>47.39651928</v>
       </c>
       <c r="G50">
-        <v>8.5444719999999901</v>
+        <v>8.4514557000000003</v>
       </c>
       <c r="H50">
-        <v>47.409101300000003</v>
+        <v>47.396457299999902</v>
       </c>
       <c r="I50">
-        <v>10442.68</v>
+        <v>8.09</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -3464,13 +3464,13 @@
         <v>47.3976112</v>
       </c>
       <c r="G51">
-        <v>8.5437472999999997</v>
+        <v>8.4507484000000002</v>
       </c>
       <c r="H51">
-        <v>47.370578599999902</v>
+        <v>47.397578899999999</v>
       </c>
       <c r="I51">
-        <v>10763.67</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -3493,13 +3493,13 @@
         <v>47.398189700000003</v>
       </c>
       <c r="G52">
-        <v>8.4365950999999999</v>
+        <v>8.4504623999999993</v>
       </c>
       <c r="H52">
-        <v>47.353817999999997</v>
+        <v>47.398172099999996</v>
       </c>
       <c r="I52">
-        <v>5122.21</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -3522,13 +3522,13 @@
         <v>47.398441779999999</v>
       </c>
       <c r="G53">
-        <v>8.5445236999999992</v>
+        <v>8.4505920999999997</v>
       </c>
       <c r="H53">
-        <v>47.372174000000001</v>
+        <v>47.3984168</v>
       </c>
       <c r="I53">
-        <v>10827.71</v>
+        <v>13.29</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -3551,13 +3551,13 @@
         <v>47.398376599999999</v>
       </c>
       <c r="G54">
-        <v>8.4513049999999996</v>
+        <v>8.4512929000000003</v>
       </c>
       <c r="H54">
-        <v>47.398335000000003</v>
+        <v>47.398347700000002</v>
       </c>
       <c r="I54">
-        <v>7.85</v>
+        <v>8.35</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -3580,13 +3580,13 @@
         <v>47.398547860000001</v>
       </c>
       <c r="G55">
-        <v>8.7873477999999992</v>
+        <v>8.4514681999999901</v>
       </c>
       <c r="H55">
-        <v>47.322698099999997</v>
+        <v>47.398508100000001</v>
       </c>
       <c r="I55">
-        <v>38277.599999999999</v>
+        <v>4.88</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -3638,13 +3638,13 @@
         <v>47.410595809999997</v>
       </c>
       <c r="G57">
-        <v>8.5272062999999996</v>
+        <v>8.4510740999999996</v>
       </c>
       <c r="H57">
-        <v>47.391000599999998</v>
+        <v>47.410573900000003</v>
       </c>
       <c r="I57">
-        <v>8730.81</v>
+        <v>8.0399999999999991</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -3667,13 +3667,13 @@
         <v>47.413701179999997</v>
       </c>
       <c r="G58">
-        <v>8.4553995999999998</v>
+        <v>8.4524442999999998</v>
       </c>
       <c r="H58">
-        <v>47.413703599999998</v>
+        <v>47.413145999999998</v>
       </c>
       <c r="I58">
-        <v>457.11</v>
+        <v>142.19</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -3725,13 +3725,13 @@
         <v>47.370821900000003</v>
       </c>
       <c r="G60">
-        <v>8.46755999999999</v>
+        <v>8.4522517999999902</v>
       </c>
       <c r="H60">
-        <v>47.407465500000001</v>
+        <v>47.370760699999998</v>
       </c>
       <c r="I60">
-        <v>4377.05</v>
+        <v>6.97</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -3754,13 +3754,13 @@
         <v>47.373915910000001</v>
       </c>
       <c r="G61">
-        <v>8.5162636000000003</v>
+        <v>8.4515428000000004</v>
       </c>
       <c r="H61">
-        <v>47.365152999999999</v>
+        <v>47.3738612</v>
       </c>
       <c r="I61">
-        <v>7266.28</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -3841,13 +3841,13 @@
         <v>47.395803860000001</v>
       </c>
       <c r="G64">
-        <v>8.5288597999999993</v>
+        <v>8.4515899000000001</v>
       </c>
       <c r="H64">
-        <v>47.342115</v>
+        <v>47.395853500000001</v>
       </c>
       <c r="I64">
-        <v>10427.6</v>
+        <v>5.58</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -3870,13 +3870,13 @@
         <v>47.39795917</v>
       </c>
       <c r="G65">
-        <v>8.5440077999999993</v>
+        <v>8.4520149</v>
       </c>
       <c r="H65">
-        <v>47.370620700000003</v>
+        <v>47.397999599999999</v>
       </c>
       <c r="I65">
-        <v>10661.2</v>
+        <v>6.08</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -3899,13 +3899,13 @@
         <v>47.397483919999999</v>
       </c>
       <c r="G66">
-        <v>8.5290392999999902</v>
+        <v>8.4520444000000001</v>
       </c>
       <c r="H66">
-        <v>47.374836600000002</v>
+        <v>47.397459599999998</v>
       </c>
       <c r="I66">
-        <v>8918.06</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -3928,13 +3928,13 @@
         <v>47.400500860000001</v>
       </c>
       <c r="G67">
-        <v>8.5627203999999999</v>
+        <v>8.4524054999999993</v>
       </c>
       <c r="H67">
-        <v>47.369931399999999</v>
+        <v>47.400424800000003</v>
       </c>
       <c r="I67">
-        <v>12744.08</v>
+        <v>23.62</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -4012,13 +4012,13 @@
         <v>47.410964679999999</v>
       </c>
       <c r="G70">
-        <v>8.52682029999999</v>
+        <v>8.4526310000000002</v>
       </c>
       <c r="H70">
-        <v>47.390839399999997</v>
+        <v>47.410883899999902</v>
       </c>
       <c r="I70">
-        <v>8548.27</v>
+        <v>9.9700000000000006</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -4099,13 +4099,13 @@
         <v>47.413328409999998</v>
       </c>
       <c r="G73">
-        <v>8.5803034999999994</v>
+        <v>8.4526380000000003</v>
       </c>
       <c r="H73">
-        <v>47.461526199999902</v>
+        <v>47.413339399999998</v>
       </c>
       <c r="I73">
-        <v>15125.61</v>
+        <v>34.29</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -4128,13 +4128,13 @@
         <v>47.413321740000001</v>
       </c>
       <c r="G74">
-        <v>8.5803034999999994</v>
+        <v>8.4526380000000003</v>
       </c>
       <c r="H74">
-        <v>47.461526199999902</v>
+        <v>47.413339399999998</v>
       </c>
       <c r="I74">
-        <v>15121.83</v>
+        <v>38.64</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -4157,13 +4157,13 @@
         <v>47.413615350000001</v>
       </c>
       <c r="G75">
-        <v>8.5602356999999998</v>
+        <v>8.4525918999999998</v>
       </c>
       <c r="H75">
-        <v>47.3751338</v>
+        <v>47.413699600000001</v>
       </c>
       <c r="I75">
-        <v>12690.86</v>
+        <v>13.05</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -4186,13 +4186,13 @@
         <v>47.369587869999997</v>
       </c>
       <c r="G76">
-        <v>8.5369638999999999</v>
+        <v>8.4527187000000001</v>
       </c>
       <c r="H76">
-        <v>47.399324800000002</v>
+        <v>47.369551299999998</v>
       </c>
       <c r="I76">
-        <v>9918.4</v>
+        <v>8.24</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -4244,13 +4244,13 @@
         <v>47.370820500000001</v>
       </c>
       <c r="G78">
-        <v>8.7809992000000001</v>
+        <v>8.4527549999999998</v>
       </c>
       <c r="H78">
-        <v>47.327529899999902</v>
+        <v>47.370765300000002</v>
       </c>
       <c r="I78">
-        <v>36819.83</v>
+        <v>6.08</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -4273,13 +4273,13 @@
         <v>47.371138420000001</v>
       </c>
       <c r="G79">
-        <v>8.4365668999999901</v>
+        <v>8.4525372999999995</v>
       </c>
       <c r="H79">
-        <v>47.353367499999997</v>
+        <v>47.371153999999997</v>
       </c>
       <c r="I79">
-        <v>2663.05</v>
+        <v>31.68</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -4302,13 +4302,13 @@
         <v>47.37071349</v>
       </c>
       <c r="G80">
-        <v>8.4694567999999997</v>
+        <v>8.4532699999999998</v>
       </c>
       <c r="H80">
-        <v>47.406642400000003</v>
+        <v>47.370688800000003</v>
       </c>
       <c r="I80">
-        <v>4343.59</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -4331,13 +4331,13 @@
         <v>47.373621040000003</v>
       </c>
       <c r="G81">
-        <v>8.5174662999999899</v>
+        <v>8.4528879999999997</v>
       </c>
       <c r="H81">
-        <v>47.363845900000001</v>
+        <v>47.373579499999998</v>
       </c>
       <c r="I81">
-        <v>7253.97</v>
+        <v>10.29</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
@@ -4360,13 +4360,13 @@
         <v>47.373763109999999</v>
       </c>
       <c r="G82">
-        <v>8.5168994999999992</v>
+        <v>8.4534223999999991</v>
       </c>
       <c r="H82">
-        <v>47.365125499999998</v>
+        <v>47.373826700000002</v>
       </c>
       <c r="I82">
-        <v>7119.19</v>
+        <v>8.6300000000000008</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -4534,13 +4534,13 @@
         <v>47.397057580000002</v>
       </c>
       <c r="G88">
-        <v>8.5444719999999901</v>
+        <v>8.4531756999999992</v>
       </c>
       <c r="H88">
-        <v>47.409101300000003</v>
+        <v>47.397044899999997</v>
       </c>
       <c r="I88">
-        <v>10235.41</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
@@ -4563,13 +4563,13 @@
         <v>47.397069139999999</v>
       </c>
       <c r="G89">
-        <v>8.5444195999999994</v>
+        <v>8.4539712999999992</v>
       </c>
       <c r="H89">
-        <v>47.409229600000003</v>
+        <v>47.397082900000001</v>
       </c>
       <c r="I89">
-        <v>10139.43</v>
+        <v>9.8699999999999992</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
@@ -4650,13 +4650,13 @@
         <v>47.397346329999998</v>
       </c>
       <c r="G92">
-        <v>8.5439395999999999</v>
+        <v>8.4532203999999993</v>
       </c>
       <c r="H92">
-        <v>47.4091393</v>
+        <v>47.3973054</v>
       </c>
       <c r="I92">
-        <v>10172.23</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
@@ -4737,13 +4737,13 @@
         <v>47.410963600000002</v>
       </c>
       <c r="G95">
-        <v>8.5266185999999902</v>
+        <v>8.4535991999999993</v>
       </c>
       <c r="H95">
-        <v>47.390935599999999</v>
+        <v>47.410929400000001</v>
       </c>
       <c r="I95">
-        <v>8415.6299999999992</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
@@ -4910,14 +4910,11 @@
       <c r="F101">
         <v>47.41292206</v>
       </c>
-      <c r="G101">
-        <v>8.4728414999999995</v>
-      </c>
-      <c r="H101">
-        <v>47.340960600000003</v>
-      </c>
-      <c r="I101">
-        <v>8214.49</v>
+      <c r="G101" t="s">
+        <v>46</v>
+      </c>
+      <c r="H101" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
@@ -4969,13 +4966,13 @@
         <v>47.413982330000003</v>
       </c>
       <c r="G103">
-        <v>8.5606248999999899</v>
+        <v>8.4531793999999998</v>
       </c>
       <c r="H103">
-        <v>47.374659800000003</v>
+        <v>47.413937300000001</v>
       </c>
       <c r="I103">
-        <v>12711.53</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
@@ -5085,13 +5082,13 @@
         <v>47.371232589999998</v>
       </c>
       <c r="G107">
-        <v>8.5254139999999996</v>
+        <v>8.4533173999999995</v>
       </c>
       <c r="H107">
-        <v>47.352712199999999</v>
+        <v>47.371093199999997</v>
       </c>
       <c r="I107">
-        <v>8212.39</v>
+        <v>65.48</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
@@ -5143,13 +5140,13 @@
         <v>47.373216820000003</v>
       </c>
       <c r="G109">
-        <v>8.4633872999999902</v>
+        <v>8.4535561999999995</v>
       </c>
       <c r="H109">
-        <v>47.314281100000002</v>
+        <v>47.373204899999998</v>
       </c>
       <c r="I109">
-        <v>6574.29</v>
+        <v>8.39</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
@@ -5172,13 +5169,13 @@
         <v>47.373618090000001</v>
       </c>
       <c r="G110">
-        <v>8.6280226999999901</v>
+        <v>8.4547256999999991</v>
       </c>
       <c r="H110">
-        <v>47.331492799999999</v>
+        <v>47.373589799999998</v>
       </c>
       <c r="I110">
-        <v>19819.080000000002</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
@@ -5288,13 +5285,13 @@
         <v>47.397033139999998</v>
       </c>
       <c r="G114">
-        <v>8.5440817999999901</v>
+        <v>8.4544084000000002</v>
       </c>
       <c r="H114">
-        <v>47.409823199999998</v>
+        <v>47.397079099999999</v>
       </c>
       <c r="I114">
-        <v>10065.469999999999</v>
+        <v>9.2200000000000006</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.2">
@@ -5317,13 +5314,13 @@
         <v>47.397672669999999</v>
       </c>
       <c r="G115">
-        <v>8.5236234999999994</v>
+        <v>8.4545797</v>
       </c>
       <c r="H115">
-        <v>47.354228999999997</v>
+        <v>47.397725199999996</v>
       </c>
       <c r="I115">
-        <v>9050.25</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.2">
@@ -5346,13 +5343,13 @@
         <v>47.410911280000001</v>
       </c>
       <c r="G116">
-        <v>8.5258839000000002</v>
+        <v>8.4545917999999993</v>
       </c>
       <c r="H116">
-        <v>47.391187000000002</v>
+        <v>47.4108667</v>
       </c>
       <c r="I116">
-        <v>8214.8799999999992</v>
+        <v>8.2899999999999991</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
@@ -5375,13 +5372,13 @@
         <v>47.410880280000001</v>
       </c>
       <c r="G117">
-        <v>8.5256410999999996</v>
+        <v>8.45504169999999</v>
       </c>
       <c r="H117">
-        <v>47.3913218</v>
+        <v>47.4108357</v>
       </c>
       <c r="I117">
-        <v>8135.13</v>
+        <v>8.82</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
@@ -5404,13 +5401,13 @@
         <v>47.410836400000001</v>
       </c>
       <c r="G118">
-        <v>8.5266504999999899</v>
+        <v>8.4554785999999993</v>
       </c>
       <c r="H118">
-        <v>47.391185499999999</v>
+        <v>47.410813900000001</v>
       </c>
       <c r="I118">
-        <v>8201.1</v>
+        <v>5.94</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.2">
@@ -5462,13 +5459,13 @@
         <v>47.41166715</v>
       </c>
       <c r="G120">
-        <v>8.4773619999999994</v>
+        <v>8.454739</v>
       </c>
       <c r="H120">
-        <v>47.405033499999902</v>
+        <v>47.4116389</v>
       </c>
       <c r="I120">
-        <v>2619.0300000000002</v>
+        <v>3.29</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.2">
@@ -5549,13 +5546,13 @@
         <v>47.370220369999998</v>
       </c>
       <c r="G123">
-        <v>8.4498131999999995</v>
+        <v>8.45582999999999</v>
       </c>
       <c r="H123">
-        <v>47.413575299999998</v>
+        <v>47.370234500000002</v>
       </c>
       <c r="I123">
-        <v>4819.49</v>
+        <v>19.91</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.2">
@@ -5578,13 +5575,13 @@
         <v>47.372062190000001</v>
       </c>
       <c r="G124">
-        <v>8.62587089999999</v>
+        <v>8.4555063999999902</v>
       </c>
       <c r="H124">
-        <v>47.332306600000003</v>
+        <v>47.372009400000003</v>
       </c>
       <c r="I124">
-        <v>19445.599999999999</v>
+        <v>6.18</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
@@ -5636,13 +5633,13 @@
         <v>47.373163220000002</v>
       </c>
       <c r="G126">
-        <v>8.5175067999999996</v>
+        <v>8.4553516000000002</v>
       </c>
       <c r="H126">
-        <v>47.363794499999997</v>
+        <v>47.373160899999903</v>
       </c>
       <c r="I126">
-        <v>6983.41</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
@@ -5694,13 +5691,13 @@
         <v>47.373214410000003</v>
       </c>
       <c r="G128">
-        <v>8.5167236000000006</v>
+        <v>8.4561227999999993</v>
       </c>
       <c r="H128">
-        <v>47.364585299999902</v>
+        <v>47.373169500000003</v>
       </c>
       <c r="I128">
-        <v>6809.58</v>
+        <v>5.52</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -5868,13 +5865,13 @@
         <v>47.396883750000001</v>
       </c>
       <c r="G134">
-        <v>8.6933480999999997</v>
+        <v>8.4563120999999999</v>
       </c>
       <c r="H134">
-        <v>47.294998700000001</v>
+        <v>47.396873399999997</v>
       </c>
       <c r="I134">
-        <v>28632.15</v>
+        <v>17.34</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
@@ -5897,13 +5894,13 @@
         <v>47.397664910000003</v>
       </c>
       <c r="G135">
-        <v>8.6926687000000005</v>
+        <v>8.4565252999999991</v>
       </c>
       <c r="H135">
-        <v>47.295347900000003</v>
+        <v>47.3976361</v>
       </c>
       <c r="I135">
-        <v>28573.52</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.2">
@@ -5926,13 +5923,13 @@
         <v>47.398530870000002</v>
       </c>
       <c r="G136">
-        <v>8.4555106000000002</v>
+        <v>8.4555132000000004</v>
       </c>
       <c r="H136">
-        <v>47.398782399999902</v>
+        <v>47.398787800000001</v>
       </c>
       <c r="I136">
-        <v>31.03</v>
+        <v>31.44</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
@@ -5955,13 +5952,13 @@
         <v>47.409040830000002</v>
       </c>
       <c r="G137">
-        <v>8.5369264000000005</v>
+        <v>8.4560937000000003</v>
       </c>
       <c r="H137">
-        <v>47.369711799999997</v>
+        <v>47.409027500000001</v>
       </c>
       <c r="I137">
-        <v>9981.57</v>
+        <v>4.3899999999999997</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
@@ -5984,13 +5981,13 @@
         <v>47.408909049999998</v>
       </c>
       <c r="G138">
-        <v>8.5376143999999901</v>
+        <v>8.4563966999999902</v>
       </c>
       <c r="H138">
-        <v>47.369470100000001</v>
+        <v>47.408934899999998</v>
       </c>
       <c r="I138">
-        <v>10021.9</v>
+        <v>2.86</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
@@ -6042,13 +6039,13 @@
         <v>47.410364680000001</v>
       </c>
       <c r="G140">
-        <v>8.5267204000000003</v>
+        <v>8.4558138999999901</v>
       </c>
       <c r="H140">
-        <v>47.390887199999902</v>
+        <v>47.410334200000001</v>
       </c>
       <c r="I140">
-        <v>8170.24</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -6071,13 +6068,13 @@
         <v>47.410311829999998</v>
       </c>
       <c r="G141">
-        <v>8.5269178999999902</v>
+        <v>8.4561841999999992</v>
       </c>
       <c r="H141">
-        <v>47.390792900000001</v>
+        <v>47.410294999999998</v>
       </c>
       <c r="I141">
-        <v>8151.03</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -6100,13 +6097,13 @@
         <v>47.410302190000003</v>
       </c>
       <c r="G142">
-        <v>8.5270341999999992</v>
+        <v>8.4566870999999999</v>
       </c>
       <c r="H142">
-        <v>47.390728699999997</v>
+        <v>47.4102636</v>
       </c>
       <c r="I142">
-        <v>8115.08</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -6129,13 +6126,13 @@
         <v>47.411668179999999</v>
       </c>
       <c r="G143">
-        <v>8.4686886999999995</v>
+        <v>8.4561978999999994</v>
       </c>
       <c r="H143">
-        <v>47.395009799999997</v>
+        <v>47.411707100000001</v>
       </c>
       <c r="I143">
-        <v>2303.25</v>
+        <v>7.09</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.2">
@@ -6158,13 +6155,13 @@
         <v>47.41118676</v>
       </c>
       <c r="G144">
-        <v>8.7039867999999991</v>
+        <v>8.4562933999999998</v>
       </c>
       <c r="H144">
-        <v>47.4895681</v>
+        <v>47.411157499999902</v>
       </c>
       <c r="I144">
-        <v>28871.19</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -6216,13 +6213,13 @@
         <v>47.411964009999998</v>
       </c>
       <c r="G146">
-        <v>8.7048577999999992</v>
+        <v>8.4558716999999994</v>
       </c>
       <c r="H146">
-        <v>47.490602000000003</v>
+        <v>47.411970799999999</v>
       </c>
       <c r="I146">
-        <v>29020.94</v>
+        <v>7.52</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.2">
@@ -6390,13 +6387,13 @@
         <v>47.37079301</v>
       </c>
       <c r="G152">
-        <v>8.4405359000000004</v>
+        <v>8.4569258999999999</v>
       </c>
       <c r="H152">
-        <v>47.403280700000003</v>
+        <v>47.370764600000001</v>
       </c>
       <c r="I152">
-        <v>4011.42</v>
+        <v>3.87</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.2">
@@ -6506,13 +6503,13 @@
         <v>47.398137890000001</v>
       </c>
       <c r="G156">
-        <v>8.5655836000000001</v>
+        <v>8.4566020000000002</v>
       </c>
       <c r="H156">
-        <v>47.285110899999999</v>
+        <v>47.398184099999902</v>
       </c>
       <c r="I156">
-        <v>17359.79</v>
+        <v>8.77</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.2">
@@ -6564,13 +6561,13 @@
         <v>47.402663230000002</v>
       </c>
       <c r="G158">
-        <v>8.4585439999999998</v>
+        <v>8.45832669999999</v>
       </c>
       <c r="H158">
-        <v>47.402548499999902</v>
+        <v>47.402603900000003</v>
       </c>
       <c r="I158">
-        <v>121.64</v>
+        <v>97.03</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.2">
@@ -6593,13 +6590,13 @@
         <v>47.408297679999997</v>
       </c>
       <c r="G159">
-        <v>8.5385229000000002</v>
+        <v>8.45768279999999</v>
       </c>
       <c r="H159">
-        <v>47.368472699999998</v>
+        <v>47.408284899999998</v>
       </c>
       <c r="I159">
-        <v>9998.44</v>
+        <v>4.57</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.2">
@@ -6709,13 +6706,13 @@
         <v>47.370233460000001</v>
       </c>
       <c r="G163">
-        <v>8.4396585000000002</v>
+        <v>8.4582082999999901</v>
       </c>
       <c r="H163">
-        <v>47.356261099999998</v>
+        <v>47.370167299999999</v>
       </c>
       <c r="I163">
-        <v>2559.86</v>
+        <v>17.97</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.2">
@@ -6738,13 +6735,13 @@
         <v>47.369853059999997</v>
       </c>
       <c r="G164">
-        <v>8.4394305999999997</v>
+        <v>8.4583295999999901</v>
       </c>
       <c r="H164">
-        <v>47.356037800000003</v>
+        <v>47.369864399999997</v>
       </c>
       <c r="I164">
-        <v>2606.7600000000002</v>
+        <v>15.66</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
@@ -6796,13 +6793,13 @@
         <v>47.37274017</v>
       </c>
       <c r="G166">
-        <v>8.5248364999999993</v>
+        <v>8.4583016000000004</v>
       </c>
       <c r="H166">
-        <v>47.352513100000003</v>
+        <v>47.372776299999998</v>
       </c>
       <c r="I166">
-        <v>7726.28</v>
+        <v>4.34</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">
@@ -6825,13 +6822,13 @@
         <v>47.373229860000002</v>
       </c>
       <c r="G167">
-        <v>8.51725759999999</v>
+        <v>8.4577524999999998</v>
       </c>
       <c r="H167">
-        <v>47.364550000000001</v>
+        <v>47.373140999999997</v>
       </c>
       <c r="I167">
-        <v>6691.02</v>
+        <v>10.49</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.2">
@@ -6970,13 +6967,13 @@
         <v>47.397314780000002</v>
       </c>
       <c r="G172">
-        <v>8.5288643999999998</v>
+        <v>8.4588536999999899</v>
       </c>
       <c r="H172">
-        <v>47.339101599999999</v>
+        <v>47.397307499999997</v>
       </c>
       <c r="I172">
-        <v>10085.23</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.2">
@@ -7057,13 +7054,13 @@
         <v>47.407519059999998</v>
       </c>
       <c r="G175">
-        <v>8.5224469000000003</v>
+        <v>8.4592720000000003</v>
       </c>
       <c r="H175">
-        <v>47.394303499999999</v>
+        <v>47.407551299999902</v>
       </c>
       <c r="I175">
-        <v>7178.03</v>
+        <v>4.24</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.2">
@@ -7086,13 +7083,13 @@
         <v>47.408161319999998</v>
       </c>
       <c r="G176">
-        <v>8.5388722999999995</v>
+        <v>8.4583288999999997</v>
       </c>
       <c r="H176">
-        <v>47.367844699999999</v>
+        <v>47.408117300000001</v>
       </c>
       <c r="I176">
-        <v>9991.8700000000008</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.2">
@@ -7115,13 +7112,13 @@
         <v>47.407738600000002</v>
       </c>
       <c r="G177">
-        <v>8.5271480000000004</v>
+        <v>8.4585708999999998</v>
       </c>
       <c r="H177">
-        <v>47.359331599999997</v>
+        <v>47.407611500000002</v>
       </c>
       <c r="I177">
-        <v>9298.25</v>
+        <v>15.04</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.2">
@@ -7143,14 +7140,11 @@
       <c r="F178">
         <v>47.407774660000001</v>
       </c>
-      <c r="G178">
-        <v>8.5271480000000004</v>
-      </c>
-      <c r="H178">
-        <v>47.359331599999997</v>
-      </c>
-      <c r="I178">
-        <v>9287.1299999999992</v>
+      <c r="G178" t="s">
+        <v>46</v>
+      </c>
+      <c r="H178" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.2">
@@ -7173,13 +7167,13 @@
         <v>47.407683030000001</v>
       </c>
       <c r="G179">
-        <v>8.5224644999999999</v>
+        <v>8.4592729999999996</v>
       </c>
       <c r="H179">
-        <v>47.394427800000003</v>
+        <v>47.4076053</v>
       </c>
       <c r="I179">
-        <v>7190.78</v>
+        <v>15.22</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.2">
@@ -7318,13 +7312,13 @@
         <v>47.412383550000001</v>
       </c>
       <c r="G184">
-        <v>8.5607293999999996</v>
+        <v>8.45901969999999</v>
       </c>
       <c r="H184">
-        <v>47.299734600000001</v>
+        <v>47.412365800000003</v>
       </c>
       <c r="I184">
-        <v>16791.919999999998</v>
+        <v>18.649999999999999</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.2">
@@ -7347,13 +7341,13 @@
         <v>47.41288788</v>
       </c>
       <c r="G185">
-        <v>8.5660834000000001</v>
+        <v>8.4586316000000004</v>
       </c>
       <c r="H185">
-        <v>47.366480099999997</v>
+        <v>47.412855</v>
       </c>
       <c r="I185">
-        <v>12993.47</v>
+        <v>4.87</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.2">
@@ -7376,13 +7370,13 @@
         <v>47.412804700000002</v>
       </c>
       <c r="G186">
-        <v>8.5661316999999997</v>
+        <v>8.4588550999999992</v>
       </c>
       <c r="H186">
-        <v>47.366384500000002</v>
+        <v>47.412762999999998</v>
       </c>
       <c r="I186">
-        <v>12977.64</v>
+        <v>4.8499999999999996</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.2">
@@ -7405,13 +7399,13 @@
         <v>47.412872640000003</v>
       </c>
       <c r="G187">
-        <v>8.5664505000000002</v>
+        <v>8.459441</v>
       </c>
       <c r="H187">
-        <v>47.366832600000002</v>
+        <v>47.412910799999999</v>
       </c>
       <c r="I187">
-        <v>12935.47</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.2">
@@ -7550,13 +7544,13 @@
         <v>47.369640959999998</v>
       </c>
       <c r="G192">
-        <v>8.5179099999999899</v>
+        <v>8.4588897999999997</v>
       </c>
       <c r="H192">
-        <v>47.363110200000001</v>
+        <v>47.369604899999999</v>
       </c>
       <c r="I192">
-        <v>6601.91</v>
+        <v>4.49</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">
@@ -7608,13 +7602,13 @@
         <v>47.370262650000001</v>
       </c>
       <c r="G194">
-        <v>8.5225738</v>
+        <v>8.4590084000000001</v>
       </c>
       <c r="H194">
-        <v>47.311509399999998</v>
+        <v>47.370269399999998</v>
       </c>
       <c r="I194">
-        <v>9572.58</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.2">
@@ -7666,13 +7660,13 @@
         <v>47.370842269999997</v>
       </c>
       <c r="G196">
-        <v>8.5179481999999993</v>
+        <v>8.4586389999999998</v>
       </c>
       <c r="H196">
-        <v>47.363719699999997</v>
+        <v>47.371028299999999</v>
       </c>
       <c r="I196">
-        <v>6622.79</v>
+        <v>29.09</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.2">
@@ -7695,13 +7689,13 @@
         <v>47.370558260000003</v>
       </c>
       <c r="G197">
-        <v>8.5181091000000002</v>
+        <v>8.4594912000000004</v>
       </c>
       <c r="H197">
-        <v>47.3635029</v>
+        <v>47.370589000000002</v>
       </c>
       <c r="I197">
-        <v>6546.77</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.2">
@@ -7724,13 +7718,13 @@
         <v>47.371161309999998</v>
       </c>
       <c r="G198">
-        <v>8.5680946000000002</v>
+        <v>8.4598192999999995</v>
       </c>
       <c r="H198">
-        <v>47.363821100000003</v>
+        <v>47.371125799999902</v>
       </c>
       <c r="I198">
-        <v>12065.36</v>
+        <v>6.45</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.2">
@@ -7811,13 +7805,13 @@
         <v>47.406258280000003</v>
       </c>
       <c r="G201">
-        <v>8.5800173999999991</v>
+        <v>8.4596970999999996</v>
       </c>
       <c r="H201">
-        <v>47.531673499999997</v>
+        <v>47.406225300000003</v>
       </c>
       <c r="I201">
-        <v>19217.3</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.2">
@@ -7840,13 +7834,13 @@
         <v>47.40664761</v>
       </c>
       <c r="G202">
-        <v>8.5233524999999997</v>
+        <v>8.4598645000000001</v>
       </c>
       <c r="H202">
-        <v>47.394215299999999</v>
+        <v>47.406664599999999</v>
       </c>
       <c r="I202">
-        <v>7199.43</v>
+        <v>6.83</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.2">
@@ -7869,13 +7863,13 @@
         <v>47.40734767</v>
       </c>
       <c r="G203">
-        <v>8.5227681000000004</v>
+        <v>8.4598151999999995</v>
       </c>
       <c r="H203">
-        <v>47.394641</v>
+        <v>47.407546500000002</v>
       </c>
       <c r="I203">
-        <v>7118.48</v>
+        <v>31.28</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.2">
@@ -7927,13 +7921,13 @@
         <v>47.406697809999997</v>
       </c>
       <c r="G205">
-        <v>8.5232159000000003</v>
+        <v>8.4599329999999995</v>
       </c>
       <c r="H205">
-        <v>47.394257600000003</v>
+        <v>47.406780900000001</v>
       </c>
       <c r="I205">
-        <v>7117.42</v>
+        <v>55.11</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.2">
@@ -7956,13 +7950,13 @@
         <v>47.406724799999999</v>
       </c>
       <c r="G206">
-        <v>8.5231221999999995</v>
+        <v>8.4599741000000002</v>
       </c>
       <c r="H206">
-        <v>47.394455600000001</v>
+        <v>47.406852499999999</v>
       </c>
       <c r="I206">
-        <v>7101.82</v>
+        <v>53.46</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.2">
@@ -7985,13 +7979,13 @@
         <v>47.408247629999998</v>
       </c>
       <c r="G207">
-        <v>8.5221003</v>
+        <v>8.4598431999999999</v>
       </c>
       <c r="H207">
-        <v>47.394362000000001</v>
+        <v>47.408319800000001</v>
       </c>
       <c r="I207">
-        <v>7083.92</v>
+        <v>10.98</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.2">
@@ -8014,13 +8008,13 @@
         <v>47.407649880000001</v>
       </c>
       <c r="G208">
-        <v>8.5224644999999999</v>
+        <v>8.4598557999999997</v>
       </c>
       <c r="H208">
-        <v>47.394427800000003</v>
+        <v>47.407591099999998</v>
       </c>
       <c r="I208">
-        <v>7095.03</v>
+        <v>20.67</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.2">
@@ -8043,13 +8037,13 @@
         <v>47.408811069999999</v>
       </c>
       <c r="G209">
-        <v>8.6204004999999899</v>
+        <v>8.4597386999999902</v>
       </c>
       <c r="H209">
-        <v>47.389299399999999</v>
+        <v>47.408479399999997</v>
       </c>
       <c r="I209">
-        <v>18004.78</v>
+        <v>36.979999999999997</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.2">
@@ -8072,13 +8066,13 @@
         <v>47.408705689999998</v>
       </c>
       <c r="G210">
-        <v>8.5214777000000002</v>
+        <v>8.4600735999999994</v>
       </c>
       <c r="H210">
-        <v>47.394543900000002</v>
+        <v>47.408587599999997</v>
       </c>
       <c r="I210">
-        <v>6991.56</v>
+        <v>19.239999999999998</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.2">
@@ -8101,13 +8095,13 @@
         <v>47.41136272</v>
       </c>
       <c r="G211">
-        <v>8.5324610999999901</v>
+        <v>8.45953119999999</v>
       </c>
       <c r="H211">
-        <v>47.368242199999997</v>
+        <v>47.411398800000001</v>
       </c>
       <c r="I211">
-        <v>9396.27</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.2">
@@ -8130,13 +8124,13 @@
         <v>47.411498969999997</v>
       </c>
       <c r="G212">
-        <v>8.5386009000000005</v>
+        <v>8.4603538999999994</v>
       </c>
       <c r="H212">
-        <v>47.366817099999999</v>
+        <v>47.411454499999998</v>
       </c>
       <c r="I212">
-        <v>9992.25</v>
+        <v>6.15</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.2">
@@ -8159,13 +8153,13 @@
         <v>47.411765840000001</v>
       </c>
       <c r="G213">
-        <v>8.5593428999999901</v>
+        <v>8.4605975000000004</v>
       </c>
       <c r="H213">
-        <v>47.302072799999998</v>
+        <v>47.4117222</v>
       </c>
       <c r="I213">
-        <v>16315.58</v>
+        <v>5.23</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.2">
@@ -8188,13 +8182,13 @@
         <v>47.411868689999999</v>
       </c>
       <c r="G214">
-        <v>8.5599857999999998</v>
+        <v>8.4604283999999996</v>
       </c>
       <c r="H214">
-        <v>47.300573300000003</v>
+        <v>47.411885599999998</v>
       </c>
       <c r="I214">
-        <v>16502.64</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.2">
@@ -8304,13 +8298,13 @@
         <v>47.369986189999999</v>
       </c>
       <c r="G218">
-        <v>8.5213035000000001</v>
+        <v>8.460737</v>
       </c>
       <c r="H218">
-        <v>47.362983</v>
+        <v>47.369957300000003</v>
       </c>
       <c r="I218">
-        <v>6783.56</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.2">
@@ -8333,13 +8327,13 @@
         <v>47.37105202</v>
       </c>
       <c r="G219">
-        <v>8.5683844999999899</v>
+        <v>8.4606253000000002</v>
       </c>
       <c r="H219">
-        <v>47.3634731</v>
+        <v>47.371037700000002</v>
       </c>
       <c r="I219">
-        <v>12009.5</v>
+        <v>5.73</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.2">
@@ -8362,13 +8356,13 @@
         <v>47.371648370000003</v>
       </c>
       <c r="G220">
-        <v>8.5248364999999993</v>
+        <v>8.4602188999999992</v>
       </c>
       <c r="H220">
-        <v>47.352513100000003</v>
+        <v>47.372633399999998</v>
       </c>
       <c r="I220">
-        <v>7430.98</v>
+        <v>124.28</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.2">
@@ -8420,13 +8414,13 @@
         <v>47.372744279999999</v>
       </c>
       <c r="G222">
-        <v>8.5248364999999993</v>
+        <v>8.4602188999999992</v>
       </c>
       <c r="H222">
-        <v>47.352513100000003</v>
+        <v>47.372633399999998</v>
       </c>
       <c r="I222">
-        <v>7437.56</v>
+        <v>91.47</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.2">
@@ -8449,13 +8443,13 @@
         <v>47.396180469999997</v>
       </c>
       <c r="G223">
-        <v>8.5433252</v>
+        <v>8.4605347000000002</v>
       </c>
       <c r="H223">
-        <v>47.410972399999999</v>
+        <v>47.395999400000001</v>
       </c>
       <c r="I223">
-        <v>9335.08</v>
+        <v>25.94</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.2">
@@ -8478,13 +8472,13 @@
         <v>47.397077600000003</v>
       </c>
       <c r="G224">
-        <v>8.4608717000000002</v>
+        <v>8.4608531999999901</v>
       </c>
       <c r="H224">
-        <v>47.397161399999902</v>
+        <v>47.397168499999999</v>
       </c>
       <c r="I224">
-        <v>23.39</v>
+        <v>21.86</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.2">
@@ -8536,13 +8530,13 @@
         <v>47.400778649999999</v>
       </c>
       <c r="G226">
-        <v>8.5629288999999993</v>
+        <v>8.4615268999999902</v>
       </c>
       <c r="H226">
-        <v>47.354291600000003</v>
+        <v>47.400776200000003</v>
       </c>
       <c r="I226">
-        <v>12386.8</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.2">
@@ -8565,13 +8559,13 @@
         <v>47.400741889999999</v>
       </c>
       <c r="G227">
-        <v>8.5628747999999995</v>
+        <v>8.4616059000000003</v>
       </c>
       <c r="H227">
-        <v>47.354465400000002</v>
+        <v>47.400748499999999</v>
       </c>
       <c r="I227">
-        <v>12356.93</v>
+        <v>4.55</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.2">
@@ -8594,13 +8588,13 @@
         <v>47.406343229999997</v>
       </c>
       <c r="G228">
-        <v>8.5236234999999994</v>
+        <v>8.4606317000000004</v>
       </c>
       <c r="H228">
-        <v>47.354228999999997</v>
+        <v>47.406295299999996</v>
       </c>
       <c r="I228">
-        <v>9053.02</v>
+        <v>5.28</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.2">
@@ -8681,13 +8675,13 @@
         <v>47.407069069999999</v>
       </c>
       <c r="G231">
-        <v>8.5439317999999993</v>
+        <v>8.4618219999999997</v>
       </c>
       <c r="H231">
-        <v>47.369417499999997</v>
+        <v>47.407016599999999</v>
       </c>
       <c r="I231">
-        <v>10059.52</v>
+        <v>34.67</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.2">
@@ -8884,13 +8878,13 @@
         <v>47.411661240000001</v>
       </c>
       <c r="G238">
-        <v>8.5387202999999996</v>
+        <v>8.4610985999999997</v>
       </c>
       <c r="H238">
-        <v>47.366438600000002</v>
+        <v>47.411591899999998</v>
       </c>
       <c r="I238">
-        <v>9995.6</v>
+        <v>36.61</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.2">
@@ -8913,13 +8907,13 @@
         <v>47.395543259999997</v>
       </c>
       <c r="G239">
-        <v>8.5433252</v>
+        <v>8.4627774999999996</v>
       </c>
       <c r="H239">
-        <v>47.410972399999999</v>
+        <v>47.395538999999999</v>
       </c>
       <c r="I239">
-        <v>9114.16</v>
+        <v>4.6100000000000003</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.2">
@@ -9000,13 +8994,13 @@
         <v>47.406199039999997</v>
       </c>
       <c r="G242">
-        <v>8.5281571999999901</v>
+        <v>8.4629732000000004</v>
       </c>
       <c r="H242">
-        <v>47.386603899999997</v>
+        <v>47.4064032</v>
       </c>
       <c r="I242">
-        <v>7613.26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.2">
@@ -9203,13 +9197,13 @@
         <v>47.41214815</v>
       </c>
       <c r="G249">
-        <v>8.5671176999999901</v>
+        <v>8.4615213999999899</v>
       </c>
       <c r="H249">
-        <v>47.3656966</v>
+        <v>47.412313599999997</v>
       </c>
       <c r="I249">
-        <v>12720.61</v>
+        <v>97.98</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.2">
@@ -9261,13 +9255,13 @@
         <v>47.392524600000002</v>
       </c>
       <c r="G251">
-        <v>8.5548001999999901</v>
+        <v>8.4647746999999995</v>
       </c>
       <c r="H251">
-        <v>47.374465099999902</v>
+        <v>47.392624900000001</v>
       </c>
       <c r="I251">
-        <v>10287.93</v>
+        <v>81.53</v>
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.2">
@@ -9435,13 +9429,13 @@
         <v>47.405746180000001</v>
       </c>
       <c r="G257">
-        <v>8.5248364999999993</v>
+        <v>8.4631603000000002</v>
       </c>
       <c r="H257">
-        <v>47.352513100000003</v>
+        <v>47.405798900000001</v>
       </c>
       <c r="I257">
-        <v>8995.02</v>
+        <v>33.159999999999997</v>
       </c>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.2">
@@ -9464,13 +9458,13 @@
         <v>47.405792300000002</v>
       </c>
       <c r="G258">
-        <v>8.5248364999999993</v>
+        <v>8.46335809999999</v>
       </c>
       <c r="H258">
-        <v>47.352513100000003</v>
+        <v>47.405752100000001</v>
       </c>
       <c r="I258">
-        <v>9013.86</v>
+        <v>10.76</v>
       </c>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.2">
@@ -9580,13 +9574,13 @@
         <v>47.411089629999999</v>
       </c>
       <c r="G262">
-        <v>8.4639287999999997</v>
+        <v>8.4639074999999995</v>
       </c>
       <c r="H262">
-        <v>47.410887899999999</v>
+        <v>47.410892399999902</v>
       </c>
       <c r="I262">
-        <v>49.59</v>
+        <v>47.25</v>
       </c>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.2">
@@ -9696,13 +9690,13 @@
         <v>47.395170280000002</v>
       </c>
       <c r="G266">
-        <v>8.55403149999999</v>
+        <v>8.4654358999999992</v>
       </c>
       <c r="H266">
-        <v>47.3750669</v>
+        <v>47.395317499999997</v>
       </c>
       <c r="I266">
-        <v>10101.01</v>
+        <v>16.260000000000002</v>
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.2">
@@ -9725,13 +9719,13 @@
         <v>47.395806149999999</v>
       </c>
       <c r="G267">
-        <v>8.5536732999999998</v>
+        <v>8.4653338999999992</v>
       </c>
       <c r="H267">
-        <v>47.3745434</v>
+        <v>47.395792899999996</v>
       </c>
       <c r="I267">
-        <v>10112.67</v>
+        <v>12.56</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.2">
@@ -9754,13 +9748,13 @@
         <v>47.39577448</v>
       </c>
       <c r="G268">
-        <v>8.5536732999999998</v>
+        <v>8.4653338999999992</v>
       </c>
       <c r="H268">
-        <v>47.3745434</v>
+        <v>47.395792899999996</v>
       </c>
       <c r="I268">
-        <v>10094.07</v>
+        <v>6.16</v>
       </c>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.2">
@@ -9812,13 +9806,13 @@
         <v>47.406391380000002</v>
       </c>
       <c r="G270">
-        <v>8.4651490000000003</v>
+        <v>8.4651589999999999</v>
       </c>
       <c r="H270">
-        <v>47.406405499999998</v>
+        <v>47.4063838</v>
       </c>
       <c r="I270">
-        <v>5.39</v>
+        <v>4.13</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.2">
@@ -9840,14 +9834,11 @@
       <c r="F271">
         <v>47.412962800000003</v>
       </c>
-      <c r="G271">
-        <v>8.5559411999999995</v>
-      </c>
-      <c r="H271">
-        <v>47.302555599999998</v>
-      </c>
-      <c r="I271">
-        <v>15791.99</v>
+      <c r="G271" t="s">
+        <v>46</v>
+      </c>
+      <c r="H271" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.2">
@@ -9957,13 +9948,13 @@
         <v>47.409339459999998</v>
       </c>
       <c r="G275">
-        <v>8.4666610999999996</v>
+        <v>8.4666595000000004</v>
       </c>
       <c r="H275">
-        <v>47.409298999999997</v>
+        <v>47.409302799999999</v>
       </c>
       <c r="I275">
-        <v>4.83</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.2">
@@ -10276,13 +10267,13 @@
         <v>47.39887547</v>
       </c>
       <c r="G286">
-        <v>8.4043127999999996</v>
+        <v>8.4668136999999994</v>
       </c>
       <c r="H286">
-        <v>47.3937217</v>
+        <v>47.399385500000001</v>
       </c>
       <c r="I286">
-        <v>7040.76</v>
+        <v>86.57</v>
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.2">
@@ -10392,13 +10383,13 @@
         <v>47.407670709999998</v>
       </c>
       <c r="G290">
-        <v>8.4608717000000002</v>
+        <v>8.4673482999999994</v>
       </c>
       <c r="H290">
-        <v>47.397161399999902</v>
+        <v>47.407719999999998</v>
       </c>
       <c r="I290">
-        <v>1364.16</v>
+        <v>6.48</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.2">
@@ -10450,13 +10441,13 @@
         <v>47.40860009</v>
       </c>
       <c r="G292">
-        <v>8.5116546999999994</v>
+        <v>8.4674855999999998</v>
       </c>
       <c r="H292">
-        <v>47.397964899999998</v>
+        <v>47.4086626</v>
       </c>
       <c r="I292">
-        <v>5044.1000000000004</v>
+        <v>9.39</v>
       </c>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.2">
@@ -10653,13 +10644,13 @@
         <v>47.395046710000003</v>
       </c>
       <c r="G299">
-        <v>8.4681820999999999</v>
+        <v>8.4681619999999995</v>
       </c>
       <c r="H299">
-        <v>47.395169899999999</v>
+        <v>47.395176399999997</v>
       </c>
       <c r="I299">
-        <v>16.66</v>
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.2">
@@ -10710,14 +10701,11 @@
       <c r="F301">
         <v>47.400290550000001</v>
       </c>
-      <c r="G301">
-        <v>8.7305659000000002</v>
-      </c>
-      <c r="H301">
-        <v>47.492276099999998</v>
-      </c>
-      <c r="I301">
-        <v>30812.66</v>
+      <c r="G301" t="s">
+        <v>46</v>
+      </c>
+      <c r="H301" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.2">
@@ -10740,13 +10728,13 @@
         <v>47.400667820000002</v>
       </c>
       <c r="G302">
-        <v>8.46709759999999</v>
+        <v>8.4822761</v>
       </c>
       <c r="H302">
-        <v>47.399905399999902</v>
+        <v>47.396522300000001</v>
       </c>
       <c r="I302">
-        <v>183.78</v>
+        <v>1591.53</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.2">
@@ -10885,13 +10873,13 @@
         <v>47.407549430000003</v>
       </c>
       <c r="G307">
-        <v>8.4594483999999994</v>
+        <v>8.4684916999999995</v>
       </c>
       <c r="H307">
-        <v>47.397750899999998</v>
+        <v>47.407433500000003</v>
       </c>
       <c r="I307">
-        <v>1474.92</v>
+        <v>12.77</v>
       </c>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.2">
@@ -10914,13 +10902,13 @@
         <v>47.407449479999997</v>
       </c>
       <c r="G308">
-        <v>8.4594483999999994</v>
+        <v>8.4684916999999995</v>
       </c>
       <c r="H308">
-        <v>47.397750899999998</v>
+        <v>47.407433500000003</v>
       </c>
       <c r="I308">
-        <v>1470.42</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.2">
@@ -11958,13 +11946,13 @@
         <v>47.4062938</v>
       </c>
       <c r="G344">
-        <v>8.7108621999999993</v>
+        <v>8.47188699999999</v>
       </c>
       <c r="H344">
-        <v>47.494459199999902</v>
+        <v>47.406242900000002</v>
       </c>
       <c r="I344">
-        <v>28293.05</v>
+        <v>5.83</v>
       </c>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.2">
@@ -11987,13 +11975,13 @@
         <v>47.407039830000002</v>
       </c>
       <c r="G345">
-        <v>8.5126831999999997</v>
+        <v>8.4708951999999993</v>
       </c>
       <c r="H345">
-        <v>47.397714099999902</v>
+        <v>47.407025300000001</v>
       </c>
       <c r="I345">
-        <v>4756.32</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.2">
@@ -12016,13 +12004,13 @@
         <v>47.406876750000002</v>
       </c>
       <c r="G346">
-        <v>8.5132867000000001</v>
+        <v>8.4716070999999999</v>
       </c>
       <c r="H346">
-        <v>47.397569300000001</v>
+        <v>47.406839099999999</v>
       </c>
       <c r="I346">
-        <v>4746.82</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.2">
@@ -12306,13 +12294,13 @@
         <v>47.390393279999998</v>
       </c>
       <c r="G356">
-        <v>8.4726944</v>
+        <v>8.472664</v>
       </c>
       <c r="H356">
-        <v>47.390340899999998</v>
+        <v>47.390296900000003</v>
       </c>
       <c r="I356">
-        <v>7.08</v>
+        <v>12.99</v>
       </c>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.2">
@@ -12625,13 +12613,13 @@
         <v>47.406288089999997</v>
       </c>
       <c r="G367">
-        <v>8.4530704999999902</v>
+        <v>8.4724862999999999</v>
       </c>
       <c r="H367">
-        <v>47.370916800000003</v>
+        <v>47.406215000000003</v>
       </c>
       <c r="I367">
-        <v>4453.3900000000003</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="368" spans="1:9" x14ac:dyDescent="0.2">
@@ -13118,13 +13106,13 @@
         <v>47.406426940000003</v>
       </c>
       <c r="G384">
-        <v>8.5146438999999994</v>
+        <v>8.47375819999999</v>
       </c>
       <c r="H384">
-        <v>47.397730299999999</v>
+        <v>47.4063971</v>
       </c>
       <c r="I384">
-        <v>4644.25</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="385" spans="1:9" x14ac:dyDescent="0.2">
@@ -13176,13 +13164,13 @@
         <v>47.406283610000003</v>
       </c>
       <c r="G386">
-        <v>8.5151763999999996</v>
+        <v>8.4743652999999899</v>
       </c>
       <c r="H386">
-        <v>47.397860199999997</v>
+        <v>47.406274699999997</v>
       </c>
       <c r="I386">
-        <v>4638.2700000000004</v>
+        <v>5.44</v>
       </c>
     </row>
     <row r="387" spans="1:9" x14ac:dyDescent="0.2">
@@ -13698,13 +13686,13 @@
         <v>47.405138729999997</v>
       </c>
       <c r="G404">
-        <v>8.7895553999999994</v>
+        <v>8.4750858000000004</v>
       </c>
       <c r="H404">
-        <v>47.321096999999902</v>
+        <v>47.4051708</v>
       </c>
       <c r="I404">
-        <v>36182.57</v>
+        <v>5.28</v>
       </c>
     </row>
     <row r="405" spans="1:9" x14ac:dyDescent="0.2">
@@ -14307,13 +14295,13 @@
         <v>47.406383259999998</v>
       </c>
       <c r="G425">
-        <v>8.5179364</v>
+        <v>8.4763687000000001</v>
       </c>
       <c r="H425">
-        <v>47.398733999999997</v>
+        <v>47.406409600000003</v>
       </c>
       <c r="I425">
-        <v>4705.0200000000004</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="426" spans="1:9" x14ac:dyDescent="0.2">
@@ -14336,13 +14324,13 @@
         <v>47.405815099999998</v>
       </c>
       <c r="G426">
-        <v>8.5172106000000003</v>
+        <v>8.4766615999999999</v>
       </c>
       <c r="H426">
-        <v>47.398219099999999</v>
+        <v>47.4058043</v>
       </c>
       <c r="I426">
-        <v>4590.9799999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="427" spans="1:9" x14ac:dyDescent="0.2">
@@ -15496,13 +15484,13 @@
         <v>47.385467419999998</v>
       </c>
       <c r="G466">
-        <v>8.4788350000000001</v>
+        <v>8.4788411000000004</v>
       </c>
       <c r="H466">
-        <v>47.385474100000003</v>
+        <v>47.385476500000003</v>
       </c>
       <c r="I466">
-        <v>1.2</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="467" spans="1:9" x14ac:dyDescent="0.2">
@@ -17120,13 +17108,13 @@
         <v>47.412465070000003</v>
       </c>
       <c r="G522">
-        <v>8.4807404999999996</v>
+        <v>8.4807965999999997</v>
       </c>
       <c r="H522">
-        <v>47.412477899999999</v>
+        <v>47.412475299999997</v>
       </c>
       <c r="I522">
-        <v>6.56</v>
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="523" spans="1:9" x14ac:dyDescent="0.2">
@@ -18425,13 +18413,13 @@
         <v>47.401631590000001</v>
       </c>
       <c r="G567">
-        <v>8.4800687000000003</v>
+        <v>8.4806302000000002</v>
       </c>
       <c r="H567">
-        <v>47.398139</v>
+        <v>47.3990133</v>
       </c>
       <c r="I567">
-        <v>419.03</v>
+        <v>306.49</v>
       </c>
     </row>
     <row r="568" spans="1:9" x14ac:dyDescent="0.2">
@@ -18947,13 +18935,13 @@
         <v>47.376138480000002</v>
       </c>
       <c r="G585">
-        <v>8.4825596999999995</v>
+        <v>8.4825549999999996</v>
       </c>
       <c r="H585">
-        <v>47.376157599999999</v>
+        <v>47.376158199999999</v>
       </c>
       <c r="I585">
-        <v>5.51</v>
+        <v>5.0599999999999996</v>
       </c>
     </row>
     <row r="586" spans="1:9" x14ac:dyDescent="0.2">
@@ -19991,13 +19979,13 @@
         <v>47.39909857</v>
       </c>
       <c r="G621">
-        <v>8.4800687000000003</v>
+        <v>8.4806302000000002</v>
       </c>
       <c r="H621">
-        <v>47.398139</v>
+        <v>47.3990133</v>
       </c>
       <c r="I621">
-        <v>335.01</v>
+        <v>255.66</v>
       </c>
     </row>
     <row r="622" spans="1:9" x14ac:dyDescent="0.2">
@@ -21470,13 +21458,13 @@
         <v>47.400836839999997</v>
       </c>
       <c r="G672">
-        <v>8.4800687000000003</v>
+        <v>8.4806302000000002</v>
       </c>
       <c r="H672">
-        <v>47.398139</v>
+        <v>47.3990133</v>
       </c>
       <c r="I672">
-        <v>469.87</v>
+        <v>362.4</v>
       </c>
     </row>
     <row r="673" spans="1:9" x14ac:dyDescent="0.2">
@@ -21557,13 +21545,13 @@
         <v>47.406707679999997</v>
       </c>
       <c r="G675">
-        <v>8.49515729999999</v>
+        <v>8.4837749999999996</v>
       </c>
       <c r="H675">
-        <v>47.402434499999998</v>
+        <v>47.406492299999996</v>
       </c>
       <c r="I675">
-        <v>1333.98</v>
+        <v>29.55</v>
       </c>
     </row>
     <row r="676" spans="1:9" x14ac:dyDescent="0.2">
@@ -22340,13 +22328,13 @@
         <v>47.382760660000002</v>
       </c>
       <c r="G702">
-        <v>8.5556488000000002</v>
+        <v>8.48468909999999</v>
       </c>
       <c r="H702">
-        <v>47.362512000000002</v>
+        <v>47.382776700000001</v>
       </c>
       <c r="I702">
-        <v>8200.1200000000008</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="703" spans="1:9" x14ac:dyDescent="0.2">
@@ -22630,13 +22618,13 @@
         <v>47.388179260000001</v>
       </c>
       <c r="G712">
-        <v>8.48524239999999</v>
+        <v>8.4853141999999995</v>
       </c>
       <c r="H712">
-        <v>47.388197499999997</v>
+        <v>47.388246100000003</v>
       </c>
       <c r="I712">
-        <v>2.67</v>
+        <v>9.6300000000000008</v>
       </c>
     </row>
     <row r="713" spans="1:9" x14ac:dyDescent="0.2">
@@ -23123,13 +23111,13 @@
         <v>47.398555999999999</v>
       </c>
       <c r="G729">
-        <v>8.4800687000000003</v>
+        <v>8.4806302000000002</v>
       </c>
       <c r="H729">
-        <v>47.398139</v>
+        <v>47.3990133</v>
       </c>
       <c r="I729">
-        <v>591.96</v>
+        <v>530.12</v>
       </c>
     </row>
     <row r="730" spans="1:9" x14ac:dyDescent="0.2">
@@ -23413,13 +23401,13 @@
         <v>47.410329560000001</v>
       </c>
       <c r="G739">
-        <v>8.5160575999999999</v>
+        <v>8.4850064999999901</v>
       </c>
       <c r="H739">
-        <v>47.361591500000003</v>
+        <v>47.410361199999997</v>
       </c>
       <c r="I739">
-        <v>6370.03</v>
+        <v>14.63</v>
       </c>
     </row>
     <row r="740" spans="1:9" x14ac:dyDescent="0.2">
@@ -25646,13 +25634,13 @@
         <v>47.384319529999999</v>
       </c>
       <c r="G816">
-        <v>8.4874610999999902</v>
+        <v>8.4875037999999901</v>
       </c>
       <c r="H816">
-        <v>47.384325699999998</v>
+        <v>47.384327999999996</v>
       </c>
       <c r="I816">
-        <v>2.2999999999999998</v>
+        <v>2.72</v>
       </c>
     </row>
     <row r="817" spans="1:9" x14ac:dyDescent="0.2">
@@ -28459,13 +28447,13 @@
         <v>47.375831759999997</v>
       </c>
       <c r="G913">
-        <v>8.5357193999999996</v>
+        <v>8.4896551000000002</v>
       </c>
       <c r="H913">
-        <v>47.321489100000001</v>
+        <v>47.375950000000003</v>
       </c>
       <c r="I913">
-        <v>7875.13</v>
+        <v>13.32</v>
       </c>
     </row>
     <row r="914" spans="1:9" x14ac:dyDescent="0.2">
@@ -29880,13 +29868,13 @@
         <v>47.369141079999999</v>
       </c>
       <c r="G962">
-        <v>8.4913717999999996</v>
+        <v>8.4913732999999993</v>
       </c>
       <c r="H962">
-        <v>47.369157899999998</v>
+        <v>47.369158400000003</v>
       </c>
       <c r="I962">
-        <v>19.2</v>
+        <v>19.04</v>
       </c>
     </row>
     <row r="963" spans="1:9" x14ac:dyDescent="0.2">
@@ -30663,13 +30651,13 @@
         <v>47.391969750000001</v>
       </c>
       <c r="G989">
-        <v>8.4914535999999998</v>
+        <v>8.4910397</v>
       </c>
       <c r="H989">
-        <v>47.392225400000001</v>
+        <v>47.392150200000003</v>
       </c>
       <c r="I989">
-        <v>28.17</v>
+        <v>48.69</v>
       </c>
     </row>
     <row r="990" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>